<commit_message>
feat: add discord bot
</commit_message>
<xml_diff>
--- a/artifacts/events.xlsx
+++ b/artifacts/events.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -817,11 +817,15 @@
 Contact:
 For questions or more information, contact
 info@bsidesmumbai.in
+Special Thanks to our Sponsors:
+HackTheBox
+Altered Security
 Follow us on social media:
 - LinkedIn: https://in.linkedin.com/company/bsidesmumbai
 - Twitter: https://twitter.com/BSidesMumbai
 - Instagram: https://www.instagram.com/bsidesmumbai/
-- Discord: https://discord.gg/2KRGQWBGR3</t>
+- Discord: https://discord.gg/2KRGQWBGR3
+Spea</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1631,6 +1635,544 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2304</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>idekCTF 2024</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2024-06-15T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2024-06-17T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">idekCTF is an information security CTF competition organized by the idek team and is aimed at the entire spectrum from high school and university students to experienced players. idekCTF will cover the standard Jeopardy-style CTF topics (binary exploitation, reverse engineering, cryptography, web exploitation, and forensics) as well as other, less standard categories. </t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://ctf.idek.team/</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>idek</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>48</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2342</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>justCTF 2024</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2024-06-15T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2024-06-16T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Sponsors: TBA</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>http://2024.justctf.team/</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>justCatTheFish</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>24</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2296</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Google Capture The Flag 2024</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2024-06-21T18:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2024-06-23T18:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>categories: web, pwn, crypto, sandbox, reversing, misc</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://g.co/ctf</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Google CTF</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>48</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2275</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>UIUCTF 2024</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2024-06-29T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2024-07-01T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>UIUCTF will be returning in 2024!</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://uiuc.tf/</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>SIGPwny</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>48</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2259</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Junior.Crypt.2024 CTF</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2024-07-03T15:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2024-07-05T15:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Junior.Crypt.2024 CTF is an open competition in information security for beginners, students and everyone. This is a 48 hour online event. We hope all participants can use their skills and have a great time.
+The organizers of the CTF were students of the Department of System Programming and Computer Security of Grodno State University, Grodno, Belarus.
+Team participation. Team of 1-4 people.
+The tasks relate to different areas - beginner, cryptography, forensics, miscellaneous, OSINT, ppc, pwn, rev, web. They will be of interest to beginners, students and everyone else.
+The official languages of the tournament are English and Russian. But you can take part even if you don't speak any of them. We will do our best to ensure that each condition of the problem can be understood with the correct use of machine translation. In addition, during the tournament tasks, we will try to introduce our participants to an unusually beautiful country, our Republic of Belarus.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>http://ctf-spcs.mf.grsu.by/</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Beavers0</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>48</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2284</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DownUnderCTF 2024</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2024-07-05T09:30:00+00:00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2024-07-07T09:30:00+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>DownUnderCTF is the largest online Australian-run Capture The Flag (CTF) competition, now welcoming Aotearoa (New Zealand) to the competition for the first time in 2024. With over 4200+ registered users and more than 2000+ registered teams as of 2023, its primary goal is to up-skill the next generation of potential Cyber Security Professionals and to expand the CTF community in Australia and Aotearoa (New Zealand). While our CTF is an online event open to participants worldwide, starting from 2024, prize eligibility extends to include both Australian and Aotearoa (New Zealand) Secondary or Tertiary school students. This change aims to foster a closer collaboration and competition spirit between the two nations while maintaining our commitment to enhancing cybersecurity skills among the youth.</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://play.duc.tf/</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>DownUnderCTF</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>48</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2301</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Interlogica CTF2024 - Wastelands</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2024-07-05T12:37:00+00:00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2024-07-07T22:59:59+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Welcome to wastelands, where the faint echoes of civilization cling to the sands like whispers of a bygone era. Abandoned technology and rusting drones dot the barren landscape, serving as eerie reminders of humanity's downfall. Amidst the desolation, the remnants of once-thriving sustainability systems cling desperately to survival, struggling to eke out existence amidst the chaos.
+Prepare to confront the harsh realities of this unforgiving terrain as you embark on thrilling challenges that will push you to your limits: Reviving Relics, Hydrophonic Systems, Unlocking the Vault, Digital Infiltration, Satellite Takeover, Expeditions, Vehicle Restoration are some of the challenges that await you!
+Embark on this epic odyssey and prove your mettle in a world where survival demands more than just strength of arms—it demands cunning, resilience, and the indomitable will to endure. Join us in the ultimate test of endurance and strategy amidst the ruins of civilization. Will you rise to the challenge, or be swallowed by the sands of time?
+Event Start:  2024 July 5 12:37
+Event End: 2024 July 7 22:59
+Maximum Team size: 5 members
+Rulez:
+1. During brute-force attacks on services and/or web pages, the use of the specified wordlists is mandatory.
+2. Actions that overload the resources of competition services, such as saturating disk space or CPU, are prohibited. These activities will be constantly monitored.
+3. Exchange of flags and/or solutions between different teams is strictly prohibited. Publishing of walkthroughs or flags before the end of the event is prohibited. Once the event has ended, publishing is encouraged.
+4. Performing attacks on infrastructures other than those specified by the challenges is prohibited.
+5. The use of multiple environments and different types of automatic encoding presupposes that the participant is able to handle them independently. In case of uncertainty, it is recommended to use a Kali/Parrot virtual machine.
+6. Each violation will result in a loss of points for the entire team.
+7. The team that first solves a specific challenge will receive additional points (first blood).
+8. The top 3 ranked teams will be awarded.
+9. Registrations on our platform will open one month before the event.
+10. Teams can consist of up to a maximum of 5 participants.
+11. If an individual does not have a team, a dedicated section for team formation will be available on Discord.
+12. Each team will be provided with a dedicated WireGuard VPN to tackle the challenges. </t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://ctf.interlogica.it/</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Interlogica</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>58</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2345</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>HITCON CTF 2024 Quals</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2024-07-12T14:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2024-07-14T14:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>TBA</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>http://ctf.hitcon.org/</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>HITCON</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>48</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2293</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MOCA CTF - Qualification</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2024-07-20T09:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2024-07-21T09:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>[DELAYED TO 20-21 July]
+Official CTF competition of the Metro Olografix Camp, organized by MOCA, Fibonhack and PWNX.
+Best teams will be invited to compete at the final events with travel expenses reinbursement!</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://moca.camp/ctf/</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Metro Olografix</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>24</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2353</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>DeadSec CTF 2024</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2024-07-26T20:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2024-07-28T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>DeadSec CTF 2024 is an online jeopardy-style CTF organized by DeadSec Team.
+There will be challenges with a wide range of difficulty mainly from cryptography, reverse, pwn, web, misc...</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>DeadSec</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>36</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2282</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>corCTF 2024</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2024-07-27T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2024-07-29T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Infra sponsored by &lt;a href="https://goo.gle/ctfsponsorship"&gt;goo.gle/ctfsponsorship&lt;/a&gt;</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://ctf.cor.team/</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Crusaders of Rust</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>48</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: improve bot methods
</commit_message>
<xml_diff>
--- a/artifacts/events.xlsx
+++ b/artifacts/events.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,37 +492,40 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2252</v>
+        <v>2259</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BYUCTF 2024</t>
+          <t>Junior.Crypt.2024 CTF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-05-17T00:00:00+00:00</t>
+          <t>2024-07-03T15:00:00+00:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-05-19T00:00:00+00:00</t>
+          <t>2024-07-05T15:00:00+00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BYUCTF will be held for its third year in a row! Going for a full 48 hours, we will have beginner- and intermediate-level challenges in a variety of categories, including web, rev, pwn, OSINT, crypto, forensics, misc, and IoT. There is no team size limit. 
-Discord link - https://discord.gg/Fe6896KEZk</t>
+          <t>Junior.Crypt.2024 CTF is an open competition in information security for beginners, students and everyone. This is a 48 hour online event. We hope all participants can use their skills and have a great time.
+The organizers of the CTF were students of the Department of System Programming and Computer Security of Grodno State University, Grodno, Belarus.
+Team participation. Team of 1-4 people.
+The tasks relate to different areas - beginner, cryptography, forensics, miscellaneous, OSINT, ppc, pwn, rev, web. They will be of interest to beginners, students and everyone else.
+The official languages of the tournament are English and Russian. But you can take part even if you don't speak any of them. We will do our best to ensure that each condition of the problem can be understood with the correct use of machine translation. In addition, during the tournament tasks, we will try to introduce our participants to an unusually beautiful country, our Republic of Belarus.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://ctfd.cyberjousting.com/</t>
+          <t>http://ctf-spcs.mf.grsu.by/</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>BYU Cyberia</t>
+          <t>Beavers0</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -540,44 +543,40 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2135</v>
+        <v>2284</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Black Cell SecOps 2024 - Online Blue Teaming Jeopardy CTF</t>
+          <t>DownUnderCTF 2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-05-17T09:00:00+00:00</t>
+          <t>2024-07-05T09:30:00+00:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-05-19T18:00:00+00:00</t>
+          <t>2024-07-07T09:30:00+00:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Our event will feature an online Jeopardy-style contest where participants can test their cybersecurity skills and compete for prizes. The CTF will be hosted in a Microsoft Azure cloud environment, where participants’ forensic investigation skills and Microsoft Sentinel knowledge will be put to the test. Participants will be provided a disk image containing forensics tools and data exports (PCAPs, memory images, disk images, etc.) collected from compromised infrastructure. Additionally, participants will be provided access to a Microsoft Sentinel instance that also contains a variety of logs from the compromised infrastructure. Using these tools and data sources contestants will need to find flags and build a timeline of the attackers’ actions…
-Scenario
-ACME is a small company with 5-10 employees working in the financial services sector. They operate a hybrid infrastructure with some resources in the cloud and some on-premises. Notably cybersecurity was never a high priority at the company, and they do not follow any on-premises or cloud security frameworks. A few weeks ago, they had suffered a ransomware attack which left their infrastructure in shambles. The IT person at the company has attempted to investigate the root cause of the attack but has found themselves in over their head. The IT person has provided you with a few data files that they had collected during their failed investigation (VM images, PCAPs, memory images, etc.) and has also given you access to their security tools. Using these tools build a timeline of the attacker’s actions and identify the traces they have left behind.
-Registration: https://blackcell.io/ctf/
-</t>
+          <t>DownUnderCTF is the largest online Australian-run Capture The Flag (CTF) competition, now welcoming Aotearoa (New Zealand) to the competition for the first time in 2024. With over 4200+ registered users and more than 2000+ registered teams as of 2023, its primary goal is to up-skill the next generation of potential Cyber Security Professionals and to expand the CTF community in Australia and Aotearoa (New Zealand). While our CTF is an online event open to participants worldwide, starting from 2024, prize eligibility extends to include both Australian and Aotearoa (New Zealand) Secondary or Tertiary school students. This change aims to foster a closer collaboration and competition spirit between the two nations while maintaining our commitment to enhancing cybersecurity skills among the youth.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://blackcell.io/ctf/</t>
+          <t>https://play.duc.tf/</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Black Cell Secops</t>
+          <t>DownUnderCTF</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -591,40 +590,72 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2289</v>
+        <v>2301</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Break the Syntax CTF 2024</t>
+          <t>Interlogica CTF2024 - Wastelands</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-05-17T16:00:00+00:00</t>
+          <t>2024-07-05T12:37:00+00:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-05-19T10:00:00+00:00</t>
+          <t>2024-07-07T22:59:59+00:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>On-site and online editions are held simultanously, on the same range of challenges so online participation is also possible. Prizes only for on-site participants.</t>
+          <t>Welcome to wastelands, where the faint echoes of civilization cling to the sands like whispers of a bygone era. Abandoned technology and rusting drones dot the barren landscape, serving as eerie reminders of humanity's downfall. Amidst the desolation, the remnants of once-thriving sustainability systems cling desperately to survival, struggling to eke out existence amidst the chaos.
+Prepare to confront the harsh realities of this unforgiving terrain as you embark on thrilling challenges that will push you to your limits: Reviving Relics, Hydrophonic Systems, Unlocking the Vault, Digital Infiltration, Satellite Takeover, Expeditions, Vehicle Restoration are some of the challenges that await you!
+Embark on this epic odyssey and prove your mettle in a world where survival demands more than just strength of arms—it demands cunning, resilience, and the indomitable will to endure. Join us in the ultimate test of endurance and strategy amidst the ruins of civilization. Will you rise to the challenge, or be swallowed by the sands of time?
+Event Start:  2024 July 5 12:37
+Event End: 2024 July 7 22:59
+Maximum Team size: 5 members
+Rulez:
+1. During brute-force attacks on services and/or web pages, the use of the specified wordlists is mandatory.
+2. Actions that overload the resources of competition services, such as saturating disk space or CPU, are prohibited. These activities will be constantly monitored.
+3. Exchange of flags and/or solutions between different teams is strictly prohibited. Publishing of walkthroughs or flags before the end of the event is prohibited. Once the event has ended, publishing is encouraged.
+4. Performing attacks on infrastructures other than those specified by the challenges is prohibited.
+5. The use of multiple environments and different types of automatic encoding presupposes that the participant is able to handle them independently. In case of uncertainty, it is recommended to use a Kali/Parrot virtual machine.
+6. Each violation will result in a loss of points for the entire team.
+7. The team that first solves a specific challenge will receive additional points (first blood).
+8. The top 3 ranked teams will be awarded.
+9. Registrations will open one month before the event.
+10. Teams can consist of up to a maximum of 5 participants.
+11. If an individual does not have a team, a dedicated section for team formation will be available on Discord.
+12. Each team will be provided with a dedicated WireGuard VPN to tackle some challenges.
+13. A maximum number of 70 teams can participate in the event.
+14. A maximum of 3 instances can be executed simultaneously by each team.
+15. The portal is integrated with our Discord server, each team will be granted private text and voice channels.
+Partecipate to our demo chall while waiting for the main event! https://ctfdemo.interlogica.ninja/ 
+If the max number of teams is reached try finding new friends and join other teams in our discord! https://discord.com/invite/DMKdECJn4y
+Main Sponsor:
+DataFlow Security (https://dfsec.com/)
+Platinum Sponsors:
+4ISP (https://www.4isp.it/)
+DV Cyber Security (https://www.dvcybersecurity.it/)
+Gold Sponsor:
+KarryCar (https://karrycar.it/)
+Silver Sponsor:
+Result Consulting (https://www.resultconsulting.it/)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://bts2024.wh.edu.pl/</t>
+          <t>https://ctf.interlogica.ninja/</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>PWr Synt@x Err0r</t>
+          <t>Interlogica</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -638,48 +669,46 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2318</v>
+        <v>2345</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VulnX CTF 2024</t>
+          <t>HITCON CTF 2024 Quals</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-05-18T10:30:00+00:00</t>
+          <t>2024-07-12T14:00:00+00:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-05-19T10:30:00+00:00</t>
+          <t>2024-07-14T14:00:00+00:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>A 24hr long CTF to test your ultimate CTF skills just before VULNCON 2024 Security conference.
-This CTF is based on a real world theme.
-More info will be added soon!</t>
+          <t>TBA</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://vulncon.in/</t>
+          <t>https://ctf2024.hitcon.org/</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>N00B_4rMY</t>
+          <t>HITCON</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="b">
         <v>0</v>
@@ -687,42 +716,50 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2299</v>
+        <v>2416</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SAS CTF 2024 Quals</t>
+          <t>OSCTF</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-05-18T12:00:00+00:00</t>
+          <t>2024-07-13T00:30:00+00:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-05-19T12:00:00+00:00</t>
+          <t>2024-07-13T16:30:00+00:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SAS CTF is an international competition for cybersecurity experts, held as a part of the Security Analyst Summit conference. The competition consists of an online Jeopardy qualification stage and on-site Attack-Defense finals.
-The qualification stage will begin on May 18 at 12:00 UTC and will last for 24 hours.
-Top 8 teams from the qualification stage will compete for a share of the $18.000 prize pot at SAS 2024 in Bali, Indonesia on October 22-25.</t>
+          <t>This exciting Capture the Flag competition will test your skills in various areas of cybersecurity and exploitation. Participants will face a series of challenges designed to push their knowledge to the limit. This CTF competition aims at school and college students, OS CTF offers something for everyone. Join us for a day of intense problem-solving, collaboration, and fun as you race against the clock and your peers to capture the flag!
+Event Type: Jeopardy, Team
+Max-Team Size: 4
+Location: Online
+Eligible: All eligible to participate but only School/College students eligible for prizes, we would require proof at the end of the event.
+Timings: 6am IST to 10pm IST
+Socials: 
+     Instagram: https://www.instagram.com/os.ctf2k24/
+     Discord: https://discord.com/invite/cPSS6pTK7T
+Sponsors: (As of 18th June 2024, any updates will be mentioned on website):
+Platinum Sponsor: Altered Security</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://ctf.thesascon.com/</t>
+          <t>https://ctf.os.ftp.sh/</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>SAS CREW</t>
+          <t>OSCTF</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -736,43 +773,55 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2315</v>
+        <v>2414</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HTB Business CTF 2024: The Vault Of Hope</t>
+          <t>CatTheQuest</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-05-18T13:00:00+00:00</t>
+          <t>2024-07-15T00:00:00+00:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-05-22T13:00:00+00:00</t>
+          <t>2024-07-21T00:00:00+00:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>In the aftermath of a devastating nuclear fallout, society’s remnants struggle amid desolation. Guided by a visionary leader, a determined group sets forth on a perilous quest to secure humanity’s future. Their target: a hidden underground vault, rumored to cradle the gold reserves of a long-forgotten nation. With promises of a new currency and societal rebirth, the team journeys through peril, each step fraught with danger.
-As daylight flickers in the wasteland, our survivors embark on gathering crucial intelligence. Through scavengers and informants, they infiltrate abandoned nuclear facilities, unveiling blueprints and schematics that decrypt the vault’s mysteries.
-Armed with this knowledge, the team maneuvers through the intricate dance of defying the vault’s formidable defenses. Skilled hackers exploit vulnerabilities, disabling sensors and outsmarting turrets. Resourceful engineers craft makeshift devices, disrupting surveillance and silencing communication frequencies, ensuring stealth amidst chaos.
-Unlock the secrets within, heralding a new era. The Vault awaits, and your journey into the unknown begins.</t>
+          <t>Prepare yourself for CatTheQuest 2024: Registrations Are Now Open!
+Dear CTF enthusiasts,
+We are thrilled to announce the opening of registrations for the very first edition of CatTheQuest, our highly anticipated Capture the Flag (CTF) competition, taking place from July 15th to July 21st, 2024, online at https://catthequest.com!
+CatTheQuest: A Virtual Odyssey
+Whether you're a seasoned veteran or a curious novice, CatTheQuest is the perfect event to test your skills, collaborate with experts, and solve security puzzles.
+An Enriching Experience
+Tiered Systems: Tailored for all levels, our challenges allow everyone to progress at their own pace, whether you're a beginner or an expert.
+Exciting Innovations: Expect numerous surprises that will make every step of this adventure even more exhilarating.
+Register Now!
+Don't miss your chance to participate in this unprecedented competition. Join us on the event's website https://catthequest.com to register and stay updated with the latest news. Connect with fellow enthusiasts, exchange tips, and prepare together to dominate the world of CatTheQuest.
+Join Our Community
+Follow us on social media to stay updated on announcements, tips, and direct interactions with organizers and other participants. Your engagement and community spirit drive our success, and we look forward to seeing you shine in this competition.
+We are eager to welcome you and celebrate this extraordinary journey together.
+See you soon at CatTheQuest!
+With enthusiasm,
+The CatTheFlag Team</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://ctf.hackthebox.com/event/details/htb-business-ctf-2024-the-vault-of-hope-1474</t>
+          <t>https://catthequest.com/</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hack The Box</t>
+          <t>CatTheFlag</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -786,66 +835,47 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2369</v>
+        <v>2396</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BSides Mumbai CTF 2024</t>
+          <t>ImaginaryCTF 2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-05-19T10:30:00+00:00</t>
+          <t>2024-07-19T19:00:00+00:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-05-19T22:30:00+00:00</t>
+          <t>2024-07-21T19:00:00+00:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Join us for the inaugural BSides Mumbai Capture The Flag (CTF) competition! This online competition, a Jeopardy Style CTF, is designed for beginners, intermediate players, and all ethical hackers. All are invited to participate! So get ready to unleash your true potential and discover the hacker in you. The competition will feature a series of challenges spanning cryptography, reverse engineering, web security, and more, catering to participants of all skill levels.
-We have lot of Categories :
-1. Web
-2. Forensic
-3. Osint
-4. Crypto
-5. Network
-6. Cloud
-7. Miscellaneous
-Contact:
-For questions or more information, contact
-info@bsidesmumbai.in
-Special Thanks to our Sponsors:
-HackTheBox
-Altered Security
-Follow us on social media:
-- LinkedIn: https://in.linkedin.com/company/bsidesmumbai
-- Twitter: https://twitter.com/BSidesMumbai
-- Instagram: https://www.instagram.com/bsidesmumbai/
-- Discord: https://discord.gg/2KRGQWBGR3
-Spea</t>
+          <t>ImaginaryCTF 2024 is a cybersecurity CTF competition run by ImaginaryCTF with a variety of challenges for all skill levels, running from July 19 to July 21. Teams will be challenged to discover vulnerabilities in websites, crack codes, and recover information through challenges in cryptography, binary exploitation, web exploitation, forensics, reversing, and more. We hope that you will learn something new from our challenges!
+Infra sponsored by goo.gle/ctfsponsorship</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://ctf.bsidesmumbai.in/</t>
+          <t>https://2024.imaginaryctf.org/</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>DarkArmy</t>
+          <t>[sqrt (-1) + 1]</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
@@ -853,42 +883,41 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2364</v>
+        <v>2293</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NahamCon CTF 2024</t>
+          <t>MOCA CTF - Quals</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-05-23T20:00:00+00:00</t>
+          <t>2024-07-20T09:00:00+00:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-05-25T20:00:00+00:00</t>
+          <t>2024-07-21T09:00:00+00:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>The NahamCon 2024 CTF will run from May 23rd to May 25th, 2024.
-Thanks to the support from you the community and our sponsors, we are pleased to offer prizes to the winners of NahamCon CTF 2024!
-Prizes will be outlined at https://ctf.nahamcon.com/prizes</t>
+          <t>Official CTF competition of the Metro Olografix Camp, organized by MOCA, fibonhack and PWNX.
+For more information about the camp and the CTF: https://moca.camp/ctf/</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://ctf.nahamcon.com/</t>
+          <t>https://play.pwnx.io/#/event/fb765f39-bc6f-46b9-a7bc-823bc261323a</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>JohnHammond</t>
+          <t>Metro Olografix</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -902,45 +931,41 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2322</v>
+        <v>2412</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>L3akCTF 2024</t>
+          <t>ENOWARS 8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-05-24T12:00:00+00:00</t>
+          <t>2024-07-20T12:00:00+00:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-05-26T12:00:00+00:00</t>
+          <t>2024-07-20T21:00:00+00:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>L3akCTF 2024 is the inaugural CTF competition organized by team L3ak!
-This is an online, jeopardy-style competition open to teams and individuals worldwide. Participants will solve cybersecurity challenges with difficulty ranging from beginner to expert.
-Categories include crypto, web, rev, pwn, forensics, osint, hardware, and misc.
-Come battle it out against the best teams in the world and hone your hacking expertise!
-Discord: https://discord.gg/wjSVdt3a7G
-Thank you to our sponsors who are supporting this event: Zellic, OtterSec, StackIt</t>
+          <t>The 8th installation of the epic ENOWARS trilogy!
+More details on our landing page</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://ctf.l3ak.team/</t>
+          <t>https://8.enowars.com/</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>L3ak</t>
+          <t>ENOFLAG</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -954,24 +979,176 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>2381</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>pbctf 2024</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-07-20T14:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-07-21T14:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Fourth edition of pbctf!
+CTF lasts for 24h, from July 20th (Saturday) 14:00 UTC to July 21th (Sunday) 14:00 UTC.
+Official website: https://ctf.perfect.blue
+Twitter: https://twitter.com/pb_ctf
+Email: team@perfect.blue
+Discord: https://discord.gg/7mNgBEHreu
+Sponsored by Zellic
+Infra sponsored by g.co/cloud</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://ctf.perfect.blue/</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>perfect blue</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>24</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2353</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DeadSec CTF 2024</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024-07-26T20:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-07-28T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>DeadSec CTF 2024 is an online jeopardy-style CTF organized by DeadSec Team.
+There will be challenges with a wide range of difficulty mainly from cryptography, reverse, pwn, web, misc...
+Infra sponsored by goo.gle/ctfsponsorship
+Sponsors:
+1- Offensive Security (https://www.offensive-security.com/)
+2- HackTheBox (https://www.hackthebox.com/)
+3- Altered Security (https://www.alteredsecurity.com/)
+4- ctf.ae (https://ctf.ae/)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>DeadSec</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>36</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2282</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>corCTF 2024</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2024-07-27T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-07-29T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Infra sponsored by &lt;a href="https://goo.gle/ctfsponsorship"&gt;goo.gle/ctfsponsorship&lt;/a&gt;
+Prizes sponsored by RET2 Systems, OtterSec, Trail of Bits, Binary Ninja, and Research Innovations.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://ctf.cor.team/</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Crusaders of Rust</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>48</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>2223</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>CrewCTF 2024</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2024-05-24T17:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2024-05-26T17:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-08-02T17:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2024-08-04T17:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>CrewCTF is an annual cybersecurity Capture The Flag competition hosted by TheHackersCrew. The third edition, CrewCTF 2024, will start at 17:00 UTC on May 24th and run for 48 hours, ending at 17:00 UTC on May 26th.
 With intermediate to expert level challenges, our contests are great opportunities for students and professionals to pick up, practice, and master skills in cybersecurity. Challenge containerization provides safe, hands-on environments for all contestants. Our CTFs are free and open to anyone with an internet connection.
@@ -980,162 +1157,18 @@
 Discord Link :  https://discord.gg/rW3dj7GhDq</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://2024.crewc.tf/</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>thehackerscrew</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H14" t="n">
         <v>48</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2340</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BTCTF I </t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2024-05-24T20:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2024-05-26T20:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A 48 hour beginner High School capture the flag hosted by Bergen County Technical High Schools Teterboro. Challenges range from beginner to medium level. </t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>https://btcodeclub.vercel.app/</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>btcodeclub</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>48</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>2375</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ångstromCTF 2024</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2024-05-25T00:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2024-05-28T00:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Geared primarily towards high school students but with a very wide range of challenge difficulty.
-Infrastructure sponsored by goo.gle/ctfsponsorship</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>https://angstromctf.com/</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>ångstromCTF Organizers</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>72</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>2257</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> GPN CTF 2024</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2024-05-31T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2024-06-01T22:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>The GPN CTF 2024 is this year’s CTF edition organized by KITCTF. Play online or in person at the GPN.
-This is a student run jeopardy-style CTF with challenges from the categories crypto, pwn, reversing, web and misc (including some more exotic ones). Featuring both a range of easy challenges from each category and a majority of hard challenges it will be a great CTF for beginners and experienced players alike.
-Communication channels: TBA</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>https://ctf.kitctf.de/</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>KITCTF</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>36</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1149,46 +1182,50 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2350</v>
+        <v>2378</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Season IV, US Cyber Open</t>
+          <t>n00bzCTF 2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024-05-31T11:59:00+00:00</t>
+          <t>2024-08-03T01:00:00+00:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-06-09T23:59:00+00:00</t>
+          <t>2024-08-05T01:00:00+00:00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>The US Cyber Games program looks forward to welcoming competitors for our Season IV campaign. Registration is free, and the competitions -- Beginner's Game Room and Competitive CTF -- are open to everyone 15+ years old. This is an INDIVIDUAL event. Due to the Federal funding received by the US Cyber Games program, we cannot allow participation from citizens of countries sanctioned by the US government. Categories covered by the Season IV, US Cyber Open include: Crypto, Forensics, PWN, Reverse Engineering, and Web.</t>
+          <t>n00bzUnit3d is back with another CTF! 
+Description: A 48 hours CTF hosted by n00bz for n00bz. Organized with beginner friendly challenges (and some hard ones), n00bzCTF is dedicated to make cyber security more friendly and approachable for complete n00bz.
+There will also be prizes for team(s) of lower scores if we get sufficient funding from our sponsors ;)
+Team limit: 4 members
+Discord: https://discord.gg/Kze7sjpgf7</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.uscybergames.com/apply-to-play-season-4?hsCtaTracking=b8a9eb7a-183c-4113-a5d4-a4ac7b486e4f%7Cb5c8f25c-5752-4e8f-815b-82cb4d186af1</t>
+          <t>https://ctf.n00bzunit3d.xyz/</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Play Cyber</t>
+          <t>n00bzUnit3d</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>228</v>
+        <v>48</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
@@ -1196,43 +1233,42 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2248</v>
+        <v>2408</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>vsCTF 2024</t>
+          <t>CTFZone 2024 Quals</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024-05-31T16:00:00+00:00</t>
+          <t>2024-08-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-06-02T16:00:00+00:00</t>
+          <t>2024-08-11T09:00:00+00:00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>View Source's 3rd CTF, now 48-hours! Challenge difficulty ranges from beginner-friendly to hard.
-High School division winners qualify for DiceCTF finals!
-Infra sponsored by goo.gle/ctfsponsorship
-Join our Discord: https://discord.gg/mVAzUJrpyf</t>
+          <t>BI.ZONE is ready to announce the date of CTFZone quals 2024!
+The first online stage will take place on August 10 at 9 AM (UTC) and will last for 24 hours. The stage format – Jeopardy – includes several categories: web, pwn, crypto, reverse and PPC.
+TOP-10 performers will proceed to the second online Attack/Defence stage of CTFZone in November 2024.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://ctf.viewsource.me/</t>
+          <t>https://ctf.bi.zone/</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>View Source</t>
+          <t>BIZone</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -1246,24 +1282,186 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2346</v>
+        <v>2304</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Codegate CTF 2024 Preliminary</t>
+          <t>idekCTF 2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2024-06-01T01:00:00+00:00</t>
+          <t>2024-08-17T00:00:00+00:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-06-02T01:00:00+00:00</t>
+          <t>2024-08-19T00:00:00+00:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>idekCTF is an information security CTF competition organized by the idek team and is aimed at the entire spectrum from high school and university students to experienced players. idekCTF will cover the standard Jeopardy-style CTF topics (binary exploitation, reverse engineering, cryptography, web exploitation, and forensics) as well as other, less standard categories. 
+Infra sponsored by goo.gle/ctfsponsorship</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://ctf.idek.team/</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>idek</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>48</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2243</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SekaiCTF 2024</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2024-08-23T16:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2024-08-25T16:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>SekaiCTF is back for its third iteration! This year's competition will feature various categories designed to test participants' skills and incentivize learning. Our CTF will have more difficult challenges, and are catered towards intermediate and advanced players - however, there will still be beginner-friendly challenges to welcome players on the newer side.
+- Categories: Web, Crypto, Pwn, Reverse, Misc, Blockchain, and Programming (PPC).
+- Prize pool: TBA
+Winner of SekaiCTF 2024 will qualify for the 9th XCTF Finals in China. https://adworld.xctf.org.cn/
+Sponsors:
+- Trail of Bits (https://www.trailofbits.com/)
+- OtterSec (https://osec.io/)
+- Sec3 (https://www.sec3.dev/)
+- Vector 35 / Binary Ninja (https://binary.ninja/)
+- Hack The Box (https://www.hackthebox.com/)
+- Offensive Security (https://www.offensive-security.com/)
+Infra sponsored by goo.gle/ctfsponsorship
+Discord: https://discord.gg/6gk7jhCgGX</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://ctf.sekai.team/</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Project Sekai</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>48</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2387</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Block Harbor VicOne Automotive CTF - Season 2</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2024-08-24T14:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2024-09-09T02:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>The BlockHarbor automotive CTF is back for season 2, and bigger than ever. Test your hand at various automotive related challenges and think with your mind wide open.
+This CTF will be a live qualifying round online. Qualifying teams have two weeks 
+during the live competition to place. The CTF qualifying challenges are available in 
+English and Japanese language. The top 4 scoring team globally and Top 2 teams in 
+Japan will be flying to Michigan USA for an onsite 1-day final round of challenges to 
+decide the winners on October 18th 2024. Top teams will be able to speak on stage at the 2024 Auto ISAC 
+summit and be awarded their prizes.
+Want to brush up on your skills? Come visit our proving grounds where old challenges each have a hands on walk-through so you know what to expect and can learn how to be a successful car hacker. Check it out at https://vsec.blockharbor.io/theplunge under the Hackathon course.
+Prior to our qualifications starting, we are actively looking for more challenge developers, if you think you've got a great idea or want to implement a challenge, our call for challenge page can be found here: https://docs.google.com/forms/d/e/1FAIpQLSeEzxlkcUmOU-uxHPb13p_ru6QZ9droV9bqEVcJ5nt6RfjW7A/viewform</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://ctf.blockharbor.io/</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>bhctf</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>372</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2347</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Codegate CTF 2024 Finals</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2024-08-29T01:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2024-08-30T01:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t xml:space="preserve">1. CODEGATE 2024 CTF has two divisions: Junior and General.
 2. Conditions of participation for each division:
@@ -1300,175 +1498,18 @@
 </t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>http://ctf.codegate.org/</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>http://www.codegate.org/</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>CODEGATE</t>
         </is>
       </c>
-      <c r="H17" t="n">
+      <c r="H20" t="n">
         <v>24</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>2358</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>N0PSctf</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2024-06-01T08:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2024-06-02T20:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>This is the first edition of N0PSctf.
-The contest will be held online, starting on June 1st at 10:00 AM, 2024 and concluding on June 2nd, 2024, at 10:00 PM (CEST).
-N0PSctf is dedicated mainly to students enrolled in French institutions but open to everyone.
-Teams are restricted to a maximum of 3 participants.
-True to tradition, participation in the CTF remains free of charge.
-We are honoured to partner with Root-Me, EURECOM, and the International Junior of EURECOM for this event.
-For further details, please visit our website via https://www.nops.re.</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>https://ctf.nops.re/</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>NOPS</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>36</v>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2222</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Akasec CTF 2024</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2024-06-07T13:37:00+00:00</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2024-06-09T13:37:00+00:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Akasec is 1337's cyber security club located in Morocco.
-Akasec CTF 2024 is an online jeopardy-style CTF organized by AkaSec club.
-A variety of challenges will be available, Web, Pwn, Reverse, Crypto, Forensics, OSINT, Boxes...
-Sponsors for the meantime :
-1337 School : https://1337.ma/
-UM6P : https://um6p.ma/
-OffSec : https://www.offsec.com/
-SecDojo : https://sec-dojo.com/
-TryHackMe : https://tryhackme.com/</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>https://ctf.akasec.club/</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>1337 KH</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>48</v>
-      </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2274</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>BCACTF 5.0</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2024-06-07T20:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2024-06-10T20:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Welcome to BCACTF 5.0!!!
-Returning for the fifth year in a row, this highschool CTF from the Bergen County Academies presents challenges in a variety of difficulties targeting everyone from beginners to CTF veterans!
-Infra sponsored by goo.gle/ctfsponsorship.</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>https://www.bcactf.com/</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>BCACTF</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>72</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -1482,44 +1523,40 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2273</v>
+        <v>2404</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R3CTF/YUANHENGCTF 2024</t>
+          <t>CISA ICS CTF 2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2024-06-08T02:00:00+00:00</t>
+          <t>2024-08-31T17:00:00+00:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-06-10T02:00:00+00:00</t>
+          <t>2024-09-04T16:00:00+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>R3CTF 2024 is a online jeopardy-style CTF organized by r3kapig and YuanHeng lab.
-Meanwhile YuanHeng lab provided all prize!
-We welcome players from all over the world to have fun during these 48 hours.
-more info:
-https://discord.gg/zU64ekBsgA</t>
+          <t>DHS CISA's annual ICS (industrial control systems) CTF is oriented around an incident response scenario involving attacks on critical infrastructure. This year, the featured critical infrastructure sectors are city infrastructure, water purification, medical facilities, and railway.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://ctf2024.r3kapig.com/</t>
+          <t>https://ctf.cisaicsctf.com/</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>r3kapig</t>
+          <t>CISA ICSJWG</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -1533,43 +1570,41 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2365</v>
+        <v>2398</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DIVER OSINT CTF 2024</t>
+          <t>CSAW CTF Qualification Round 2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2024-06-08T03:00:00+00:00</t>
+          <t>2024-09-06T16:00:00+00:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-06-09T03:00:00+00:00</t>
+          <t>2024-09-08T16:00:00+00:00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>DIVER OSINT CTF is the real-world oriented OSINT CTF.
-We provide country/region-neutral OSINT challenges.
-Challenges will be available in English and Japanese.
-Anyone is welcome to join.</t>
+          <t>CSAW CTF is one of the oldest and biggest CTFs with 1096 teams with 1+ points in 2023. Designed as an entry-level, jeopardy-style CTF, this competition is for students who are trying to break into the field of security, as well as for advanced students and industry professionals who want to practice their skills.
+Our competition occurs over two rounds: a Qualifying Round in September and a Final Round in November.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://twitter.com/DIVER_OSINT_CTF</t>
+          <t>https://ctf.csaw.io/</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>diver_osint</t>
+          <t>NYUSEC</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -1583,43 +1618,37 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2210</v>
+        <v>2418</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Crypto CTF 2024</t>
+          <t>snakeCTF 2024 Quals</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2024-06-08T14:00:00+00:00</t>
+          <t>2024-09-07T08:00:00+00:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2024-06-09T14:00:00+00:00</t>
+          <t>2024-09-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Crypto CTF is an online competition for hackers to test, evaluate, and expand their skills in exploiting cryptography. In this CTF, we will provide various crypto challenges that focus on modern cryptography techniques.
-All crypto lovers are most welcome!
-Crypto CTF is a response to the longstanding complaints by CTF participants about the crypto challenges in CTF contests. In this brand-new tournament, we aim to provide crypto enthusiasts with fun and challenging pure crypto tasks that will truly test their passion for cryptography.
-Each task will be based on a specific cryptographic primitive or will involve a direct application of cryptography in other fields.
-The organizers of these tournaments generously offer their knowledge and skills to design original Crypto tasks and challenges for similar contests.
-Long Live Crypto :)
-Discord: https://discord.gg/RsvAJtF5Q5
-Twitter: https://twitter.com/Crypto_CTF</t>
+          <t>SnakeCTF is an online jeopardy-style CTF featuring challenges from many categories, including pwn, web, reversing, crypto, forensics and network.
+This event serves as a qualification for the Finals. We will invite the **top 8 teams from the Schengen area** to the Finals, which will be held in Lignano Sabbiadoro, Udine, Italy from 2024-12-05 to 2024-12-08.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://cr.yp.toc.tf/</t>
+          <t>https://2024.snakectf.org/</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>ASIS</t>
+          <t>MadrHacks</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1637,40 +1666,45 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2304</v>
+        <v>2410</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>idekCTF 2024</t>
+          <t xml:space="preserve"> Securinets CTF Quals 2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2024-06-15T00:00:00+00:00</t>
+          <t>2024-09-14T19:00:00+00:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-06-17T00:00:00+00:00</t>
+          <t>2024-09-15T19:00:00+00:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">idekCTF is an information security CTF competition organized by the idek team and is aimed at the entire spectrum from high school and university students to experienced players. idekCTF will cover the standard Jeopardy-style CTF topics (binary exploitation, reverse engineering, cryptography, web exploitation, and forensics) as well as other, less standard categories. </t>
+          <t>CTF Securinets Quals 2024 is an on-line jeopardy style CTF organized by Securinets Club.
+The CTF starts 19:00 UTC (20:00 in Tunisia).
+Only 15 teams will qualify to the final CTF + top 3 Tunisians.
+Registration will be open soon.
+Join our discord channel:
+https://discord.gg/VPJPKDwRj5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://ctf.idek.team/</t>
+          <t>https://ctf.securinets.tn/</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>idek</t>
+          <t>Securinets</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -1684,36 +1718,36 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2342</v>
+        <v>2411</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>justCTF 2024</t>
+          <t>Cyber Jawara International</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2024-06-15T08:00:00+00:00</t>
+          <t>2024-09-21T01:59:00+00:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2024-06-16T08:00:00+00:00</t>
+          <t>2024-09-22T01:59:00+00:00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Sponsors: TBA</t>
+          <t>The CYBER JAWARA competition was first held in 2012 organized by ID-SIRTII / CC. Since 2020 Cyber Jawara has continued to be held by CSIRT.ID. This competition is held to inspire and encourage the growth of interests, talents, and human resource potential in Cyber Security initiatives in Indonesia. We are grateful that since then similar activities - including other pre-existing Cyber Security Competition series - have begun to receive wider attention and recognition. Therefore, CYBER JAWARA has effectively become a dissemination and awareness medium of general Cyber Security issues.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>http://2024.justctf.team/</t>
+          <t>https://cyberjawara.id/2024</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>justCatTheFish</t>
+          <t>idnsa</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1731,40 +1765,40 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2296</v>
+        <v>2211</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Google Capture The Flag 2024</t>
+          <t>ASIS CTF Quals 2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2024-06-21T18:00:00+00:00</t>
+          <t>2024-09-21T14:00:00+00:00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2024-06-23T18:00:00+00:00</t>
+          <t>2024-09-22T14:00:00+00:00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>categories: web, pwn, crypto, sandbox, reversing, misc</t>
+          <t>ASIS CTF Quals 2024</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://g.co/ctf</t>
+          <t>https://asisctf.com/</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Google CTF</t>
+          <t>ASIS</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -1778,40 +1812,40 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2275</v>
+        <v>2351</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>UIUCTF 2024</t>
+          <t>FAUST CTF 2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2024-06-29T00:00:00+00:00</t>
+          <t>2024-09-28T12:00:00+00:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2024-07-01T00:00:00+00:00</t>
+          <t>2024-09-28T21:00:00+00:00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>UIUCTF will be returning in 2024!</t>
+          <t>Classic online attack-defense CTF. Each team will be given a Vulnbox image to host itself and VPN access. You will run exploits against other teams, capture flags and submit them to our server.</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://uiuc.tf/</t>
+          <t>https://2024.faustctf.net/</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>SIGPwny</t>
+          <t>FAUST</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -1825,44 +1859,42 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2259</v>
+        <v>2389</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Junior.Crypt.2024 CTF</t>
+          <t>BRICS+ CTF Quals 2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2024-07-03T15:00:00+00:00</t>
+          <t>2024-10-05T10:00:00+00:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2024-07-05T15:00:00+00:00</t>
+          <t>2024-10-06T10:00:00+00:00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Junior.Crypt.2024 CTF is an open competition in information security for beginners, students and everyone. This is a 48 hour online event. We hope all participants can use their skills and have a great time.
-The organizers of the CTF were students of the Department of System Programming and Computer Security of Grodno State University, Grodno, Belarus.
-Team participation. Team of 1-4 people.
-The tasks relate to different areas - beginner, cryptography, forensics, miscellaneous, OSINT, ppc, pwn, rev, web. They will be of interest to beginners, students and everyone else.
-The official languages of the tournament are English and Russian. But you can take part even if you don't speak any of them. We will do our best to ensure that each condition of the problem can be understood with the correct use of machine translation. In addition, during the tournament tasks, we will try to introduce our participants to an unusually beautiful country, our Republic of Belarus.</t>
+          <t>We invite you to take a participation in cybersecurity international team competitions BRICS+ Capture The Flag. The qualification stage will be online in CTF Jeopardy format. The best teams will be able to compete in the final, which will be held online in CTF Attack-Defense format.
+The CTF is for any academic/professional team from all around the world. Best teams from BRICS countries and international (all over the world) teams will be invited to the final round (Prize pool of the finals is 1 000 000 roubles). Before the final round we will ask eligible for the BRICS quota teams to verify their status.
+More information about quals: https://brics-ctf.com/</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>http://ctf-spcs.mf.grsu.by/</t>
+          <t>https://brics-ctf.com/</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Beavers0</t>
+          <t>ITMO FSIT</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -1871,305 +1903,6 @@
         <v>0</v>
       </c>
       <c r="K28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>2284</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>DownUnderCTF 2024</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>2024-07-05T09:30:00+00:00</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2024-07-07T09:30:00+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>DownUnderCTF is the largest online Australian-run Capture The Flag (CTF) competition, now welcoming Aotearoa (New Zealand) to the competition for the first time in 2024. With over 4200+ registered users and more than 2000+ registered teams as of 2023, its primary goal is to up-skill the next generation of potential Cyber Security Professionals and to expand the CTF community in Australia and Aotearoa (New Zealand). While our CTF is an online event open to participants worldwide, starting from 2024, prize eligibility extends to include both Australian and Aotearoa (New Zealand) Secondary or Tertiary school students. This change aims to foster a closer collaboration and competition spirit between the two nations while maintaining our commitment to enhancing cybersecurity skills among the youth.</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>https://play.duc.tf/</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>DownUnderCTF</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>48</v>
-      </c>
-      <c r="I29" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>2301</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Interlogica CTF2024 - Wastelands</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>2024-07-05T12:37:00+00:00</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2024-07-07T22:59:59+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Welcome to wastelands, where the faint echoes of civilization cling to the sands like whispers of a bygone era. Abandoned technology and rusting drones dot the barren landscape, serving as eerie reminders of humanity's downfall. Amidst the desolation, the remnants of once-thriving sustainability systems cling desperately to survival, struggling to eke out existence amidst the chaos.
-Prepare to confront the harsh realities of this unforgiving terrain as you embark on thrilling challenges that will push you to your limits: Reviving Relics, Hydrophonic Systems, Unlocking the Vault, Digital Infiltration, Satellite Takeover, Expeditions, Vehicle Restoration are some of the challenges that await you!
-Embark on this epic odyssey and prove your mettle in a world where survival demands more than just strength of arms—it demands cunning, resilience, and the indomitable will to endure. Join us in the ultimate test of endurance and strategy amidst the ruins of civilization. Will you rise to the challenge, or be swallowed by the sands of time?
-Event Start:  2024 July 5 12:37
-Event End: 2024 July 7 22:59
-Maximum Team size: 5 members
-Rulez:
-1. During brute-force attacks on services and/or web pages, the use of the specified wordlists is mandatory.
-2. Actions that overload the resources of competition services, such as saturating disk space or CPU, are prohibited. These activities will be constantly monitored.
-3. Exchange of flags and/or solutions between different teams is strictly prohibited. Publishing of walkthroughs or flags before the end of the event is prohibited. Once the event has ended, publishing is encouraged.
-4. Performing attacks on infrastructures other than those specified by the challenges is prohibited.
-5. The use of multiple environments and different types of automatic encoding presupposes that the participant is able to handle them independently. In case of uncertainty, it is recommended to use a Kali/Parrot virtual machine.
-6. Each violation will result in a loss of points for the entire team.
-7. The team that first solves a specific challenge will receive additional points (first blood).
-8. The top 3 ranked teams will be awarded.
-9. Registrations on our platform will open one month before the event.
-10. Teams can consist of up to a maximum of 5 participants.
-11. If an individual does not have a team, a dedicated section for team formation will be available on Discord.
-12. Each team will be provided with a dedicated WireGuard VPN to tackle the challenges. </t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>https://ctf.interlogica.it/</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Interlogica</t>
-        </is>
-      </c>
-      <c r="H30" t="n">
-        <v>58</v>
-      </c>
-      <c r="I30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>2345</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>HITCON CTF 2024 Quals</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>2024-07-12T14:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2024-07-14T14:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>TBA</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>http://ctf.hitcon.org/</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>HITCON</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>48</v>
-      </c>
-      <c r="I31" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>2293</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>MOCA CTF - Qualification</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>2024-07-20T09:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2024-07-21T09:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>[DELAYED TO 20-21 July]
-Official CTF competition of the Metro Olografix Camp, organized by MOCA, Fibonhack and PWNX.
-Best teams will be invited to compete at the final events with travel expenses reinbursement!</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>https://moca.camp/ctf/</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Metro Olografix</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>24</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>2353</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>DeadSec CTF 2024</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>2024-07-26T20:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>2024-07-28T08:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>DeadSec CTF 2024 is an online jeopardy-style CTF organized by DeadSec Team.
-There will be challenges with a wide range of difficulty mainly from cryptography, reverse, pwn, web, misc...</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>DeadSec</t>
-        </is>
-      </c>
-      <c r="H33" t="n">
-        <v>36</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>2282</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>corCTF 2024</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>2024-07-27T00:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>2024-07-29T00:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Infra sponsored by &lt;a href="https://goo.gle/ctfsponsorship"&gt;goo.gle/ctfsponsorship&lt;/a&gt;</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>https://ctf.cor.team/</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Crusaders of Rust</t>
-        </is>
-      </c>
-      <c r="H34" t="n">
-        <v>48</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" t="b">
-        <v>0</v>
-      </c>
-      <c r="K34" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>